<commit_message>
Minor changes and readme file improved
</commit_message>
<xml_diff>
--- a/selenium_tests/test_results.xlsx
+++ b/selenium_tests/test_results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Test Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Test Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -44,14 +44,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0000FF00"/>
-        <bgColor rgb="0000FF00"/>
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,9 +455,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="35" customWidth="1" min="3" max="3"/>
+    <col width="59" customWidth="1" min="3" max="3"/>
     <col width="65" customWidth="1" min="4" max="4"/>
     <col width="17" customWidth="1" min="5" max="5"/>
     <col width="15" customWidth="1" min="6" max="6"/>
@@ -510,26 +510,36 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Login Test</t>
+          <t>Test E2E</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>TCI001</t>
+          <t>TCE001</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>Interact with video inside iframe</t>
+          <t>Complete E2E test with valid data</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to home page
-    2. Switch to iframe containing video
-    3. Click play button on video
-    4. Switch back to default content
-    5. Click on Products link</t>
+2. Click login link
+3. Enter username and password
+4. Click login button
+5. Verify redirection to home page
+6. Navigate to products page
+7. Enter search text
+8. Verify if products are found
+9. Add product to cart
+10. Accept alert
+11. Navigate to cart page
+12. Click checkout
+13. Fill in checkout details
+14. Click place order
+15. Verify success message</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -539,37 +549,852 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>Invalid</t>
+          <t>Valid</t>
         </is>
       </c>
       <c r="G2" s="3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>Username: testuser1, Password: password123, Search Text: Pot, Fullname: Juan Camilo Loaiza Alarcon, Email: jcloaizaa@example.com, Address: 123 Av. Example, City: Montreal, Postalcode: 12345, Cardholder: Juan Camilo Loaiza Alarcon, Cardnumber: 12345678910111213, Expiry: 12/25, CVV: 123</t>
         </is>
       </c>
       <c r="H2" s="4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
+          <t>Test E2E</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>TCE002</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Invalid product search during E2E test</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to home page
+2. Click login link
+3. Enter username and password
+4. Click login button
+5. Verify redirection to home page
+6. Navigate to products page
+7. Enter search text
+8. Verify if products are found</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>invalid search</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Password: password123, Search Text: Lamp</t>
+        </is>
+      </c>
+      <c r="H3" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Test E2E</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>TCE003</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Invalid login attempt during E2E test</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to home page
+2. Click login link
+3. Enter username and password
+4. Click login button
+5. Verify redirection to home page</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>invalid login</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>Username: wronguser, Password: password123</t>
+        </is>
+      </c>
+      <c r="H4" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
           <t>Login Test</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>TCA001</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>valid user and password</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to login page
+2. Enter username and password
+3. Click login button
+4. Verify redirection to home page</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>valid</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>Valid</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Password: password123</t>
+        </is>
+      </c>
+      <c r="H5" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Login Test</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>TCA002</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>invalid user and password</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to login page
+2. Enter username and password
+3. Click login button
+4. Verify redirection to home page</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser2, Password: securepass</t>
+        </is>
+      </c>
+      <c r="H6" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Login Test</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>TCA003</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>valid user but invalid password</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to login page
+2. Enter username and password
+3. Click login button
+4. Verify redirection to home page</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Password: wrongpass</t>
+        </is>
+      </c>
+      <c r="H7" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Login Test</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>TCA004</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>invalid user but valid password</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to login page
+2. Enter username and password
+3. Click login button
+4. Verify redirection to home page</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser67, Password: password123</t>
+        </is>
+      </c>
+      <c r="H8" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Login Test</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>TCA005</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>different valid user and password</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to login page
+2. Enter username and password
+3. Click login button
+4. Verify redirection to home page</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>valid</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>Valid</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>Username: sampleuser, Password: mypassword</t>
+        </is>
+      </c>
+      <c r="H9" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Login Test</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>TCA006</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>valid user but valid password from another user</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to login page
+2. Enter username and password
+3. Click login button
+4. Verify redirection to home page</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>Username: sampleuser, Password: password123</t>
+        </is>
+      </c>
+      <c r="H10" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Test Reset Password</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>TCR001</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>valid user code and password</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to forgot password page
+2. Enter username, code, new password, and confirm password
+3. Click reset password button
+4. Verify redirection to login page</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>valid</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>Valid</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Code: 1234, Password: Password.123, Confirm Password: Password.123</t>
+        </is>
+      </c>
+      <c r="H11" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>Test Reset Password</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>TCR002</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>Complete E2E test with valid data</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to forgot password page
+2. Enter username, code, new password, and confirm password
+3. Click reset password button
+4. Verify redirection to login page</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G12" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Code: wrongcode, Password: Password.123, Confirm Password: Password.123</t>
+        </is>
+      </c>
+      <c r="H12" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Test Reset Password</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>TCR003</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Complete E2E test with valid data</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to forgot password page
+2. Enter username, code, new password, and confirm password
+3. Click reset password button
+4. Verify redirection to login page</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G13" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser2, Code: 1234, Password: Password.123, Confirm Password: Password.123</t>
+        </is>
+      </c>
+      <c r="H13" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Test Reset Password</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>TCR004</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>Complete E2E test with valid data</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to forgot password page
+2. Enter username, code, new password, and confirm password
+3. Click reset password button
+4. Verify redirection to login page</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G14" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Code: 5678, Password: Password.123, Confirm Password: Password.1234</t>
+        </is>
+      </c>
+      <c r="H14" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>Test Reset Password</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>TCR005</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>Complete E2E test with valid data</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to forgot password page
+2. Enter username, code, new password, and confirm password
+3. Click reset password button
+4. Verify redirection to login page</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G15" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Code: 1234, Password: Password.123, Confirm Password: Password</t>
+        </is>
+      </c>
+      <c r="H15" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>Test Reset Password</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>TCR006</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>Complete E2E test with valid data</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to forgot password page
+2. Enter username, code, new password, and confirm password
+3. Click reset password button
+4. Verify redirection to login page</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Code: 1234, Password: pass, Confirm Password: pass</t>
+        </is>
+      </c>
+      <c r="H16" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>Test Reset Password</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>TCR007</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>Complete E2E test with valid data</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to forgot password page
+2. Enter username, code, new password, and confirm password
+3. Click reset password button
+4. Verify redirection to login page</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Code: 1234, Password: password.123, Confirm Password: password.123</t>
+        </is>
+      </c>
+      <c r="H17" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Test Reset Password</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>TCR008</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>Complete E2E test with valid data</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to forgot password page
+2. Enter username, code, new password, and confirm password
+3. Click reset password button
+4. Verify redirection to login page</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G18" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Code: 1234, Password: PASSWORD.123, Confirm Password: PASSWORD.123</t>
+        </is>
+      </c>
+      <c r="H18" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>Test Reset Password</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>TCR009</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>Complete E2E test with valid data</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to forgot password page
+2. Enter username, code, new password, and confirm password
+3. Click reset password button
+4. Verify redirection to login page</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Code: 1234, Password: Password123, Confirm Password: Password123</t>
+        </is>
+      </c>
+      <c r="H19" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>Test Reset Password</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>TCR0010</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>Complete E2E test with valid data</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to forgot password page
+2. Enter username, code, new password, and confirm password
+3. Click reset password button
+4. Verify redirection to login page</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G20" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Code: 1234, Password: Password., Confirm Password: Password.</t>
+        </is>
+      </c>
+      <c r="H20" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>Login Test</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>TCI001</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C21" s="2" t="inlineStr">
         <is>
           <t>Interact with video inside iframe</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D21" s="3" t="inlineStr">
         <is>
           <t>1. Navigate to home page
 2. Switch to iframe containing video
@@ -578,22 +1403,420 @@
 5. Click on Products link</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="E21" s="2" t="inlineStr">
         <is>
           <t>valid</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G21" s="3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H21" s="5" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Login Test</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>TCI001</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>Interact with video inside iframe</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to home page
+2. Switch to iframe containing video
+3. Click play button on video
+4. Switch back to default content
+5. Click on Products link</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
         <is>
           <t>valid</t>
         </is>
       </c>
-      <c r="G3" s="3" t="inlineStr">
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>valid</t>
+        </is>
+      </c>
+      <c r="G22" s="3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="H3" s="5" t="inlineStr">
+      <c r="H22" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>Test Registration</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>TCREG001</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>valid user age and password</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to registration page
+2. Enter username, email, age, password, and confirm password
+3. Click register button</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>valid</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>Valid</t>
+        </is>
+      </c>
+      <c r="G23" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser1, Email: testuser1@example.com, Age: 25, Password: Password.123, Confirm Password: Password.123</t>
+        </is>
+      </c>
+      <c r="H23" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>Test Registration</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>TCREG002</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>valid user and password but invalid age</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to registration page
+2. Enter username, email, age, password, and confirm password
+3. Click register button</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G24" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser2, Email: testuser2@example.com, Age: 10, Password: Password.123, Confirm Password: Password.123</t>
+        </is>
+      </c>
+      <c r="H24" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>Test Registration</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>TCREG003</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
+          <t>valid user and age but passwords do not match</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to registration page
+2. Enter username, email, age, password, and confirm password
+3. Click register button</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G25" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser3, Email: testuser3@example.com, Age: 20, Password: password, Confirm Password: Password.123</t>
+        </is>
+      </c>
+      <c r="H25" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>Test Registration</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>TCREG004</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>valid user and age but password does'nt meet criteria</t>
+        </is>
+      </c>
+      <c r="D26" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to registration page
+2. Enter username, email, age, password, and confirm password
+3. Click register button</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G26" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser4, Email: testuser4@example.com, Age: 25, Password: password, Confirm Password: password</t>
+        </is>
+      </c>
+      <c r="H26" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>Test Registration</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>TCREG005</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>valid user and age but password missing uppercase letter</t>
+        </is>
+      </c>
+      <c r="D27" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to registration page
+2. Enter username, email, age, password, and confirm password
+3. Click register button</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G27" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser5, Email: testuser5@example.com, Age: 30, Password: password.123, Confirm Password: password.123</t>
+        </is>
+      </c>
+      <c r="H27" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>Test Registration</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>TCREG006</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>valid user and age but password missing lowercase letter</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to registration page
+2. Enter username, email, age, password, and confirm password
+3. Click register button</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G28" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser6, Email: testuser6@example.com, Age: 22, Password: PASSWORD.123, Confirm Password: PASSWORD.123</t>
+        </is>
+      </c>
+      <c r="H28" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>Test Registration</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>TCREG007</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t>valid user and age but password missing special character</t>
+        </is>
+      </c>
+      <c r="D29" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to registration page
+2. Enter username, email, age, password, and confirm password
+3. Click register button</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G29" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser7, Email: testuser7@example.com, Age: 25, Password: Password123, Confirm Password: Password123</t>
+        </is>
+      </c>
+      <c r="H29" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>Test Registration</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>TCREG008</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>valid user and age but password missing number</t>
+        </is>
+      </c>
+      <c r="D30" s="3" t="inlineStr">
+        <is>
+          <t>1. Navigate to registration page
+2. Enter username, email, age, password, and confirm password
+3. Click register button</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>invalid</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>Invalid</t>
+        </is>
+      </c>
+      <c r="G30" s="3" t="inlineStr">
+        <is>
+          <t>Username: testuser8, Email: testuser8@example.com, Age: 25, Password: Password., Confirm Password: Password.</t>
+        </is>
+      </c>
+      <c r="H30" s="4" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>

</xml_diff>